<commit_message>
se cambio la fecha por la de venta
</commit_message>
<xml_diff>
--- a/Tabla/new.xlsx
+++ b/Tabla/new.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,110 +458,1672 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CARIBBEAN LUMBER AGUADILLA</t>
+          <t>CARIBBEAN LUMBER 65 INFANTERIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MARGARITA SANTOS CORTES</t>
+          <t>JANNISSE HERNANDEZ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5.3046</t>
+          <t>4.9286</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>530.46</t>
+          <t>492.86</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CARIBBEAN LUMBER AGUADILLA</t>
+          <t>CARIBBEAN LUMBER ADJUNTAS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MARIANGELLYS CARRERO RAMOS</t>
+          <t>LESLIE MARIE RODRIGUEZ PACHECO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2.4127</t>
+          <t>4.8404</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>241.27</t>
+          <t>484.04</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CARIBBEAN LUMBER FAJARDO</t>
+          <t>CARIBBEAN LUMBER ADJUNTAS</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>KATTY ROLDAN GUADALUPE</t>
+          <t>MELANIE MEDINA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.360</t>
+          <t>2.0812</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>36.0</t>
+          <t>208.12</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CARIBBEAN LUMBER HUMACAO</t>
+          <t>CARIBBEAN LUMBER AGUADA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MILAGROS ROLON SIERRA</t>
+          <t>CYNTHIA DUPREY VALENTIN</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.7316</t>
+          <t>8.0794</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>173.16</t>
+          <t>807.94</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>CARIBBEAN LUMBER AGUADA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SANDRA ACEVEDO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4.9382</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>493.82</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER AGUADILLA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MARGARITA SANTOS CORTES</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>29.2212</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2922.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER AGUADILLA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MARIANGELLYS CARRERO RAMOS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2.8862</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>288.62</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER AGUASBUENA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GINNI FUENTES</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4.9114</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>491.14</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER AIBONITO</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>YAMIRA MATEO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3.7598</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>375.98</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER AIBONITO</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>YAZMIN MELENDEZ</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1.800</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>180.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER ANASCO</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>JACQUELINE CARABALLO MONSEGUR</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>5.6106</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>561.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER ANASCO</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MARIALINA VALENTIN VELEZ</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.5999</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>59.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER ARECIBO</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>LISANDRA LUGO ALAGO</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>10.2119</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1021.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER ARECIBO</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>YESENIA CORTES ORTIZ</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>26.0154</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2601.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER BARRANQUITAS</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>LYDIA PEREZ ROQUE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>6.3146</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>631.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER BAYAMON</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MICHELLE QUIROS</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>30.4646</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3046.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CABO ROJO</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MARISOL LUGO MERCADO</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14.1094</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1410.94</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CABO ROJO</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SONIA COLLADO VELEZ</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>11.0235</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1102.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CAGUAS 1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MADELINE ARROYO BARBOSA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>22.1345</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2213.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CANOVANAS</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GRACE MARIE MAISONET VEGA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2.4185</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>241.85</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CANOVANAS</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MARGARITA SANTOS VERA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>18.7179</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1871.79</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CAROLINA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CAROLINA GUZMAN SANTOS</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>5.9666</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>596.66</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CAYEY</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>VERONICA DE JESUS ORTIZ</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>24.0066</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2400.66</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CERAMICA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ALBA QUILES SANTIAGO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4.6663</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>466.63</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CERAMICA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MARICELIS HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2.4743</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>247.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CIDRA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BRENDA L ROLON HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>3.8149</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>381.49</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER COAMO</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ROSYMEL ROQUE TORRES</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1.2054</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>120.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER CUPEY</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MARY ANN UBARRI</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>11.9491</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1194.91</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER DORADO</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>EVA PEREZ CORA</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>13.9212</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1392.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER FAJARDO</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>AIDA VILLAFANE REYES</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>5.3640</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>536.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER FAJARDO</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>KATTY ROLDAN GUADALUPE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>23.8690</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2386.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER FAJARDO</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>YARALEE CRUZ</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>26.3624</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2636.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER GUAYAMA</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>JAZMIN VAZQUEZ PEREZ</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>22.6442</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2264.42</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER GUAYAMA</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>YAMIRIS GARCIA</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>60.4480</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>6044.80</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER GUAYNABO</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>JAILYN ROSARIO GARCIA</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>19.6700</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>1967.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER GUAYNABO</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SHELLY URBINA</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>9.1019</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>910.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER HATO REY</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>IRIS HERNANDEZ MALAVE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>3.0331</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>303.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER HATO REY</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>YAHAIRA ESCRIBANO</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1.9170</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>191.70</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER HATO TEJAS</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>AIMEE LUGO ROMAN</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>12.9007</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>1290.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER HUMACAO</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CARMEN VELAZQUEZ</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>9.0223</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>902.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER HUMACAO</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MILAGROS ROLON SIERRA</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>32.8879</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>3288.79</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER ISABELA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ANGEL MARRERO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>6.9123</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>691.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER ISABELA</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>LISBETHMARIE ORTIZ ROLDAN</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>37.6821</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>3768.21</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER JUANA DIAZ</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BRITNEY ANN TORRES FIGUEROA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>4.3108</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>431.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER JUNCOS</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>JEANNETTE TORRES TORRES</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>5.8869</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>588.69</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER LEVITTOWN</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>CARMEN OQUENDO VAZQUEZ</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>6.9172</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>691.72</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER MANATI</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MARIA DEL MAR RIVERA GONZALEZ</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>15.7181</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1571.81</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER MANATI</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>VANESSA TORRES CRUZ</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>15.9942</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>1599.42</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER MAYAGUEZ 1</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>KRISTANAECE CRUZ ROSADO</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>12.3985</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>1239.85</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER MAYAGUEZ 1</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MARLYN COLLAZO MONTES</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>4.8905</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>489.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER MAYAGUEZ 2</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CARMEN MOJICA</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>3.8827</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>388.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER MAYAGUEZ 2</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CARMEN RUIZ CARABALLO</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>17.4047</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1740.47</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER MOROVIS</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>JORGE BRACERO ZENO</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>8.1836</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>818.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER NARANJITO</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>CELINES NIEVES</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>23.3369</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2333.69</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER PENUELAS</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ROSA E CORDERO GUZMAN</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1.2499</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>124.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER PONCE</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>CAMILLE FRANCESCHI</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>13.0491</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>1304.91</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER PONCE</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>JUANA M PEREZ TORRES</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>7.7463</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>774.63</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER QUEBRADILLAS</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>EDITH M QUILES CRESPO</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>9.6219</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>962.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER RIO GRANDE</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ASHLEY PEREZ</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>4.8576</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>485.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER RIO GRANDE</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>EMILY CARRILLO MERCADO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.3260</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>32.60</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
           <t>CARIBBEAN LUMBER SALINAS</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B62" t="inlineStr">
         <is>
           <t>IRIS YAHAIRA FERNANDEZ CRUZ</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.0354</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3.54</t>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>4.9858</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>498.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER SAN GERMAN</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>OMAYRA OLMEDA</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>15.7762</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>1577.62</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER SAN GERMAN</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>VIRGEN FLORES OLIVENCIA</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>4.4654</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>446.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER SANTURCE</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Y ANED CRUZ</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2.0206</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>202.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER SSEBASTIAN</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>BETZAIDA RAMIREZ</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>12.3944</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>1239.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER SSEBASTIAN</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>MINERVA AVILES PEREZ</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>5.6134</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>561.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER TOA ALTA</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ANNIE MORALES RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>4.9887</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>498.87</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER TRUJILLO</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>YARELIS HERNADEZ TORRES</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>10.5490</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1054.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER UTUADO</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>JESSEIKA RIVERA RIVERA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>12.8320</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>1283.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER VICTORY</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>JESSICA REYES LOZADA</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>19.9815</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>1998.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER VICTORY</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>JOMARIE SANTIAGO</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0.1198</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>11.98</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER VILLALBA</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>GLORIMAR SANTIAGO</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>1.6337</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>163.37</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER VILLALBA</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>JESUS J BURGOS</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>1.7777</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>177.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER YABUCOA</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ALANIS F RIVERA MEDINA</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>7.1029</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>710.29</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER YAUCO</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>RUTH CARABALLO</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>14.0210</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>1402.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>CARIBBEAN LUMBER YAUCO</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>VALLERIE VAZQUEZ BATTISTINI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>18.8312</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>1883.12</t>
         </is>
       </c>
     </row>

</xml_diff>